<commit_message>
Changed scenario settings. Added scratch worksheet.
</commit_message>
<xml_diff>
--- a/benchmark_scenarios.xlsx
+++ b/benchmark_scenarios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="sketch worksheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>tp1</t>
   </si>
@@ -84,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,11 +108,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -121,6 +133,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,8 +476,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>50000000</v>
+        <v>5000000</v>
       </c>
       <c r="D4" s="1">
         <v>30</v>
@@ -603,7 +615,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>50000000</v>
+        <v>5000000</v>
       </c>
       <c r="D7" s="1">
         <v>30</v>
@@ -623,4 +635,195 @@
     <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;K000000&amp;F: &amp;A&amp;C&amp;"Calibri,Regular"&amp;K000000CONFIDENTIAL&amp;R&amp;"Calibri,Regular"&amp;K000000&amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>500000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <f>G2*C3/C2</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <f>G3*C4/C3</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>500000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <f>G2*1.5</f>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <f>G3*1.5</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="D7" s="1">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <f>G4*1.5</f>
+        <v>675</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.36000000000000004" right="0.36000000000000004" top="0.75000000000000011" bottom="0.6100000000000001" header="0.5" footer="0.39000000000000007"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;K000000&amp;F: &amp;A&amp;C&amp;"Calibri,Regular"&amp;K000000CONFIDENTIAL&amp;R&amp;"Calibri,Regular"&amp;K000000&amp;P/&amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>